<commit_message>
Updated user flow excel file
</commit_message>
<xml_diff>
--- a/Joylist100_UserFlow.xlsx
+++ b/Joylist100_UserFlow.xlsx
@@ -438,13 +438,13 @@
       <xdr:col>20</xdr:col>
       <xdr:colOff>490220</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:rowOff>33020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -453,7 +453,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17000220" y="579120"/>
+          <a:off x="17000220" y="1366520"/>
           <a:ext cx="2113280" cy="1376680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -902,13 +902,13 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>706120</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>117685</xdr:rowOff>
+      <xdr:rowOff>168485</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>520700</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>110065</xdr:rowOff>
+      <xdr:rowOff>160865</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -917,8 +917,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10662920" y="862752"/>
-          <a:ext cx="2303780" cy="2227580"/>
+          <a:off x="10612120" y="930485"/>
+          <a:ext cx="2291080" cy="2278380"/>
         </a:xfrm>
         <a:prstGeom prst="diamond">
           <a:avLst/>
@@ -1018,13 +1018,13 @@
       <xdr:col>16</xdr:col>
       <xdr:colOff>553720</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>117685</xdr:rowOff>
+      <xdr:rowOff>168485</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>110065</xdr:rowOff>
+      <xdr:rowOff>160865</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1033,8 +1033,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13829453" y="862752"/>
-          <a:ext cx="2303780" cy="2227580"/>
+          <a:off x="13761720" y="930485"/>
+          <a:ext cx="2291080" cy="2278380"/>
         </a:xfrm>
         <a:prstGeom prst="diamond">
           <a:avLst/>
@@ -1390,7 +1390,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>113875</xdr:rowOff>
+      <xdr:rowOff>164675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
@@ -1408,8 +1408,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="9207500" y="2018875"/>
-          <a:ext cx="1404620" cy="50802"/>
+          <a:off x="9207500" y="2069675"/>
+          <a:ext cx="1404620" cy="2"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1440,13 +1440,13 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>520700</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>113875</xdr:rowOff>
+      <xdr:rowOff>164675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>553720</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>113875</xdr:rowOff>
+      <xdr:rowOff>164675</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1458,8 +1458,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12966700" y="1976542"/>
-          <a:ext cx="862753" cy="0"/>
+          <a:off x="12903200" y="2069675"/>
+          <a:ext cx="858520" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1488,13 +1488,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>198543</xdr:colOff>
+      <xdr:colOff>200661</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>110064</xdr:rowOff>
+      <xdr:rowOff>160864</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
+      <xdr:colOff>203201</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>96519</xdr:rowOff>
     </xdr:to>
@@ -1508,8 +1508,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="11544511" y="3360630"/>
-          <a:ext cx="545255" cy="4657"/>
+          <a:off x="11505353" y="3461172"/>
+          <a:ext cx="507155" cy="2540"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -1878,13 +1878,13 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>113875</xdr:rowOff>
+      <xdr:rowOff>149860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>490220</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>122343</xdr:rowOff>
+      <xdr:rowOff>164675</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1895,9 +1895,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="16133233" y="1976542"/>
-          <a:ext cx="951654" cy="8468"/>
+        <a:xfrm flipV="1">
+          <a:off x="16052800" y="2054860"/>
+          <a:ext cx="947420" cy="14815"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1926,15 +1926,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>718820</xdr:colOff>
+      <xdr:colOff>718821</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>110065</xdr:rowOff>
+      <xdr:rowOff>160864</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>46143</xdr:colOff>
+      <xdr:colOff>48261</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>173143</xdr:rowOff>
+      <xdr:rowOff>175259</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1946,13 +1946,13 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="13474276" y="4440343"/>
-          <a:ext cx="2857078" cy="157056"/>
+          <a:off x="13393843" y="4567342"/>
+          <a:ext cx="2871895" cy="154940"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector4">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 38213"/>
-            <a:gd name="adj2" fmla="val 245553"/>
+            <a:gd name="adj1" fmla="val 38016"/>
+            <a:gd name="adj2" fmla="val 247541"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -2358,15 +2358,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>723477</xdr:colOff>
+      <xdr:colOff>721360</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>7619</xdr:rowOff>
+      <xdr:rowOff>33020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>122342</xdr:rowOff>
+      <xdr:rowOff>149860</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2378,13 +2378,13 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="18342610" y="1116753"/>
-          <a:ext cx="673523" cy="1062990"/>
+          <a:off x="18241010" y="1182370"/>
+          <a:ext cx="688340" cy="1056640"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector4">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -69139"/>
-            <a:gd name="adj2" fmla="val 127877"/>
+            <a:gd name="adj1" fmla="val -33210"/>
+            <a:gd name="adj2" fmla="val 121635"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -4359,8 +4359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:AI76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R20" workbookViewId="0">
-      <selection activeCell="V24" sqref="V24"/>
+    <sheetView tabSelected="1" topLeftCell="L2" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>